<commit_message>
copying cell formats when flattening
</commit_message>
<xml_diff>
--- a/_examples/spreadsheet/flatten/formulas.xlsx
+++ b/_examples/spreadsheet/flatten/formulas.xlsx
@@ -45,12 +45,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="167" formatCode="0.00%"/>
-    <numFmt numFmtId="168" formatCode="#,##0.00000000"/>
+    <numFmt numFmtId="168" formatCode="General"/>
+    <numFmt numFmtId="169" formatCode="#,##0.00000000"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -339,11 +340,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -444,16 +445,16 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -497,7 +498,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="n">
         <f aca="false" t="array" ref="B8:B10">IF(A4:A6&gt;4,B4:B6)</f>
         <v>0</v>
@@ -507,7 +508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="n">
         <v>0</v>
       </c>
@@ -516,7 +517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="n">
         <v>8</v>
       </c>
@@ -525,7 +526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <f aca="false" t="array" ref="A11:B11">IF(A4:B4&gt;5,TRUE())</f>
         <v>0</v>
@@ -559,12 +560,12 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -689,7 +690,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -785,16 +786,16 @@
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AC1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -817,18 +818,18 @@
         <v>0.061</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="5" t="n">
-        <v>0.061</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="0" t="n">
-        <f aca="false">PRICEMAT(C1,C2,C3,C4,C5,C6)</f>
-        <v>99.9802978513638</v>
+        <f aca="false">PRICEDISC(C1,C2,C4,C5,C6)</f>
+        <v>99.0172222222222</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1058,18 +1059,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
         <v>3</v>
       </c>
@@ -1084,7 +1085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <f aca="false" t="array" ref="A2:B2">IF(A1:B1&gt;5,TRUE())</f>
         <v>0</v>
@@ -1256,8 +1257,8 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="n">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1" t="n">
         <f aca="false" t="array" ref="B12:E14">IF(B6:E6&gt;2,B8:D10)</f>
         <v>0</v>
       </c>
@@ -1271,7 +1272,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="n">
         <v>0</v>
       </c>
@@ -1285,7 +1286,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="n">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
copying cell formats when flattening (#369)
</commit_message>
<xml_diff>
--- a/_examples/spreadsheet/flatten/formulas.xlsx
+++ b/_examples/spreadsheet/flatten/formulas.xlsx
@@ -45,12 +45,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="167" formatCode="0.00%"/>
-    <numFmt numFmtId="168" formatCode="#,##0.00000000"/>
+    <numFmt numFmtId="168" formatCode="General"/>
+    <numFmt numFmtId="169" formatCode="#,##0.00000000"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -339,11 +340,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -444,16 +445,16 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -497,7 +498,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="n">
         <f aca="false" t="array" ref="B8:B10">IF(A4:A6&gt;4,B4:B6)</f>
         <v>0</v>
@@ -507,7 +508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="n">
         <v>0</v>
       </c>
@@ -516,7 +517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="n">
         <v>8</v>
       </c>
@@ -525,7 +526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <f aca="false" t="array" ref="A11:B11">IF(A4:B4&gt;5,TRUE())</f>
         <v>0</v>
@@ -559,12 +560,12 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -689,7 +690,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -785,16 +786,16 @@
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AC1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -817,18 +818,18 @@
         <v>0.061</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="5" t="n">
-        <v>0.061</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="0" t="n">
-        <f aca="false">PRICEMAT(C1,C2,C3,C4,C5,C6)</f>
-        <v>99.9802978513638</v>
+        <f aca="false">PRICEDISC(C1,C2,C4,C5,C6)</f>
+        <v>99.0172222222222</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1058,18 +1059,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
         <v>3</v>
       </c>
@@ -1084,7 +1085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <f aca="false" t="array" ref="A2:B2">IF(A1:B1&gt;5,TRUE())</f>
         <v>0</v>
@@ -1256,8 +1257,8 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="n">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1" t="n">
         <f aca="false" t="array" ref="B12:E14">IF(B6:E6&gt;2,B8:D10)</f>
         <v>0</v>
       </c>
@@ -1271,7 +1272,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="n">
         <v>0</v>
       </c>
@@ -1285,7 +1286,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="n">
         <v>0</v>
       </c>

</xml_diff>